<commit_message>
Refactored Types to store vertices as vector<> making initialisation and transfer cleaner Added support for UV maps Removed redundent methods in bridge Added MaxScripts (just copied at the moment)
</commit_message>
<xml_diff>
--- a/Daz Materials.xlsx
+++ b/Daz Materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Daz Material Types" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="239">
   <si>
     <t>GlossinessValueMap</t>
   </si>
@@ -723,9 +723,6 @@
     <t>Max Type</t>
   </si>
   <si>
-    <t>MaxScript Command</t>
-  </si>
-  <si>
     <t>Conversion</t>
   </si>
   <si>
@@ -736,9 +733,6 @@
   </si>
   <si>
     <t>ColourFromString</t>
-  </si>
-  <si>
-    <t>The following are intended as guidance - not for copy &amp; pasting - converting between Daz/Max is not that simple unfortunately</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2740,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,8 +2744,8 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="2.5703125" customWidth="1"/>
-    <col min="6" max="6" width="117.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
@@ -2764,19 +2758,14 @@
         <v>234</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="10" t="s">
-        <v>240</v>
-      </c>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -2786,10 +2775,7 @@
         <v>134</v>
       </c>
       <c r="C3" s="7"/>
-      <c r="F3" s="9" t="str">
-        <f>IF(AND(D3&lt;&gt;"",C3&lt;&gt;""),CONCATENATE("myMaterial.",A3," = ",C3," (maxBridgeInstance.GetMaterialProperty myMaterialId """,D3,""")"),"")</f>
-        <v/>
-      </c>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -2799,10 +2785,7 @@
         <v>136</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="F4" s="9" t="str">
-        <f t="shared" ref="F4:F67" si="0">IF(AND(D4&lt;&gt;"",C4&lt;&gt;""),CONCATENATE("myMaterial.",A4," = ",C4," (maxBridgeInstance.GetMaterialProperty myMaterialId """,D4,""")"),"")</f>
-        <v/>
-      </c>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -2812,10 +2795,7 @@
         <v>136</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="F5" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -2825,10 +2805,7 @@
         <v>136</v>
       </c>
       <c r="C6" s="7"/>
-      <c r="F6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -2838,10 +2815,7 @@
         <v>136</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="F7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -2851,10 +2825,7 @@
         <v>141</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="F8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -2864,10 +2835,7 @@
         <v>134</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="F9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -2877,15 +2845,12 @@
         <v>144</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>myMaterial.opacity  = PercentFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "BaseOpacity")</v>
-      </c>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -2895,10 +2860,7 @@
         <v>146</v>
       </c>
       <c r="C11" s="7"/>
-      <c r="F11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2908,10 +2870,7 @@
         <v>148</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="F12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -2921,10 +2880,7 @@
         <v>134</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="F13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2934,10 +2890,7 @@
         <v>144</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="F14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -2947,10 +2900,7 @@
         <v>152</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="F15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -2960,10 +2910,7 @@
         <v>152</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="F16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -2973,10 +2920,7 @@
         <v>134</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="F17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -2986,10 +2930,7 @@
         <v>136</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="F18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -2999,10 +2940,7 @@
         <v>152</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="F19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -3012,15 +2950,12 @@
         <v>152</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>myMaterial.reflectionLevel = FloatFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "ReflectionStrength")</v>
-      </c>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -3030,10 +2965,7 @@
         <v>134</v>
       </c>
       <c r="C21" s="7"/>
-      <c r="F21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -3043,10 +2975,7 @@
         <v>152</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="F22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -3056,10 +2985,7 @@
         <v>136</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="F23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -3069,10 +2995,7 @@
         <v>152</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="F24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -3082,10 +3005,7 @@
         <v>136</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="F25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -3095,10 +3015,7 @@
         <v>136</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="F26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -3108,10 +3025,7 @@
         <v>136</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="F27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -3121,10 +3035,7 @@
         <v>141</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="F28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
@@ -3134,10 +3045,7 @@
         <v>152</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="F29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -3147,10 +3055,7 @@
         <v>152</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="F30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
@@ -3160,10 +3065,7 @@
         <v>136</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="F31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -3173,10 +3075,7 @@
         <v>170</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="F32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -3186,10 +3085,7 @@
         <v>172</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="F33" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -3199,10 +3095,7 @@
         <v>174</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="F34" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
@@ -3212,10 +3105,7 @@
         <v>136</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="F35" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
@@ -3226,10 +3116,7 @@
       <c r="D36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
@@ -3237,10 +3124,7 @@
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
-      <c r="F37" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -3248,10 +3132,7 @@
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
-      <c r="F38" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -3262,10 +3143,7 @@
       <c r="D39" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
@@ -3276,10 +3154,7 @@
       <c r="D40" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -3287,10 +3162,7 @@
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
-      <c r="F41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -3301,10 +3173,7 @@
       <c r="D42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
@@ -3315,10 +3184,7 @@
       <c r="D43" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -3326,10 +3192,7 @@
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
-      <c r="F44" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -3337,10 +3200,10 @@
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
-      <c r="F45" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="D45" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
@@ -3348,10 +3211,7 @@
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
-      <c r="F46" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
@@ -3359,10 +3219,7 @@
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
-      <c r="F47" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
@@ -3370,10 +3227,7 @@
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
-      <c r="F48" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
@@ -3381,10 +3235,7 @@
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
-      <c r="F49" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
@@ -3392,10 +3243,7 @@
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
-      <c r="F50" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
@@ -3406,10 +3254,7 @@
       <c r="D51" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F51" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -3417,10 +3262,7 @@
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
-      <c r="F52" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
@@ -3428,10 +3270,7 @@
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
-      <c r="F53" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
@@ -3439,10 +3278,10 @@
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
-      <c r="F54" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="D54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
@@ -3450,10 +3289,7 @@
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
-      <c r="F55" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
@@ -3461,10 +3297,7 @@
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
-      <c r="F56" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
@@ -3472,10 +3305,10 @@
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
-      <c r="F57" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="D57" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
@@ -3483,10 +3316,7 @@
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
-      <c r="F58" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -3494,10 +3324,7 @@
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
-      <c r="F59" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
@@ -3505,10 +3332,10 @@
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
-      <c r="F60" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="D60" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
@@ -3516,10 +3343,7 @@
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
-      <c r="F61" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F61" s="9"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
@@ -3527,10 +3351,7 @@
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
-      <c r="F62" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
@@ -3538,10 +3359,7 @@
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
-      <c r="F63" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
@@ -3549,10 +3367,7 @@
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
-      <c r="F64" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
@@ -3560,10 +3375,7 @@
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
-      <c r="F65" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -3574,10 +3386,7 @@
       <c r="D66" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F66" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
@@ -3585,10 +3394,7 @@
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
-      <c r="F67" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
@@ -3596,10 +3402,7 @@
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
-      <c r="F68" s="9" t="str">
-        <f t="shared" ref="F68:F90" si="1">IF(AND(D68&lt;&gt;"",C68&lt;&gt;""),CONCATENATE("myMaterial.",A68," = ",C68," (maxBridgeInstance.GetMaterialProperty myMaterialId """,D68,""")"),"")</f>
-        <v/>
-      </c>
+      <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
@@ -3610,10 +3413,7 @@
       <c r="D69" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F69" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
@@ -3621,10 +3421,7 @@
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="F70" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
@@ -3632,10 +3429,7 @@
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
-      <c r="F71" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
@@ -3645,10 +3439,7 @@
         <v>152</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="F72" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
@@ -3658,10 +3449,7 @@
         <v>152</v>
       </c>
       <c r="C73" s="7"/>
-      <c r="F73" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
@@ -3671,10 +3459,7 @@
         <v>152</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="F74" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
@@ -3684,10 +3469,7 @@
         <v>136</v>
       </c>
       <c r="C75" s="7"/>
-      <c r="F75" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
@@ -3697,10 +3479,7 @@
         <v>136</v>
       </c>
       <c r="C76" s="7"/>
-      <c r="F76" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F76" s="9"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
@@ -3710,10 +3489,7 @@
         <v>136</v>
       </c>
       <c r="C77" s="7"/>
-      <c r="F77" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
@@ -3723,10 +3499,7 @@
         <v>136</v>
       </c>
       <c r="C78" s="7"/>
-      <c r="F78" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
@@ -3736,15 +3509,12 @@
         <v>146</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F79" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>myMaterial.ambient = ColourFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "AmbientColor")</v>
-      </c>
+      <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
@@ -3754,15 +3524,12 @@
         <v>146</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F80" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>myMaterial.diffuse = ColourFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "DiffuseColor")</v>
-      </c>
+      <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
@@ -3772,15 +3539,12 @@
         <v>146</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F81" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>myMaterial.specular = ColourFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "SpecularColor")</v>
-      </c>
+      <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
@@ -3790,10 +3554,7 @@
         <v>136</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="F82" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F82" s="9"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
@@ -3803,10 +3564,7 @@
         <v>136</v>
       </c>
       <c r="C83" s="7"/>
-      <c r="F83" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F83" s="9"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
@@ -3816,10 +3574,7 @@
         <v>136</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="F84" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
@@ -3829,10 +3584,7 @@
         <v>136</v>
       </c>
       <c r="C85" s="7"/>
-      <c r="F85" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
@@ -3842,10 +3594,7 @@
         <v>144</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="F86" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
@@ -3855,10 +3604,7 @@
         <v>146</v>
       </c>
       <c r="C87" s="7"/>
-      <c r="F87" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F87" s="9"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
@@ -3868,15 +3614,12 @@
         <v>144</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F88" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>myMaterial.specularLevel = PercentFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "SpecularStrength")</v>
-      </c>
+      <c r="F88" s="9"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
@@ -3886,15 +3629,12 @@
         <v>144</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F89" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>myMaterial.glossiness  = PercentFromString (maxBridgeInstance.GetMaterialProperty myMaterialId "GlossinessStrength")</v>
-      </c>
+      <c r="F89" s="9"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
@@ -3904,10 +3644,7 @@
         <v>152</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="F90" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="F90" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Triangulation method to managed code to speed up import (how effective this has been remains to be seen...)
</commit_message>
<xml_diff>
--- a/Daz Materials.xlsx
+++ b/Daz Materials.xlsx
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2734,7 +2734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
About to refactor materials code to handle all materials, including DzShaderMaterial, generically.
</commit_message>
<xml_diff>
--- a/Daz Materials.xlsx
+++ b/Daz Materials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="242">
   <si>
     <t>GlossinessValueMap</t>
   </si>
@@ -733,13 +733,22 @@
   </si>
   <si>
     <t>ColourFromString</t>
+  </si>
+  <si>
+    <t>Percent multiplied with diffuse colour (from map or DiffuseColor property)</t>
+  </si>
+  <si>
+    <t>Diffuse Colour map</t>
+  </si>
+  <si>
+    <t>Diffuse Colour is multiplied with Diffuse Map (if present) and Diffuse Strength</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -788,6 +797,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -821,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -833,6 +858,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1134,24 +1162,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="96.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="39.5703125" customWidth="1"/>
-    <col min="9" max="9" width="96.85546875" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="96.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" customWidth="1"/>
+    <col min="10" max="10" width="96.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1159,698 +1188,754 @@
         <v>52</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="str">
-        <f>CONCATENATE("properties[""",B3,"""] = PropertyToString( material-&gt;",C3,A3,"() );")</f>
+      <c r="C3" s="12"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="str">
+        <f>CONCATENATE("properties[""",B3,"""] = PropertyToString( material-&gt;",D3,A3,"() );")</f>
         <v>properties["allowsAutoBake"] = PropertyToString( material-&gt;allowsAutoBake() );</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="7" t="str">
-        <f t="shared" ref="D4:D48" si="0">CONCATENATE("properties[""",B4,"""] = PropertyToString( material-&gt;",C4,A4,"() );")</f>
+      <c r="C4" s="12"/>
+      <c r="D4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="7" t="str">
+        <f t="shared" ref="E4:E48" si="0">CONCATENATE("properties[""",B4,"""] = PropertyToString( material-&gt;",D4,A4,"() );")</f>
         <v>properties["BaseOpacity"] = PropertyToString( material-&gt;getBaseOpacity() );</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="7" t="str">
+      <c r="C5" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["ColorMap"] = PropertyToString( material-&gt;getColorMap() );</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="7" t="str">
+      <c r="C6" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DiffuseColor"] = PropertyToString( material-&gt;getDiffuseColor() );</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="7" t="str">
+      <c r="C7" s="12"/>
+      <c r="D7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["MaterialType"] = PropertyToString( material-&gt;getMaterialName() );</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="7" t="str">
+      <c r="C8" s="12"/>
+      <c r="D8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["NumGLMaps"] = PropertyToString( material-&gt;getNumGLMaps() );</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="7" t="str">
+      <c r="C9" s="12"/>
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["OpacityMap"] = PropertyToString( material-&gt;getOpacityMap() );</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="str">
+      <c r="C10" s="12"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["isColorMappable"] = PropertyToString( material-&gt;isColorMappable() );</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="str">
+      <c r="C11" s="12"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["isOpacityMappable"] = PropertyToString( material-&gt;isOpacityMappable() );</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="str">
+      <c r="C12" s="12"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["isOpaque"] = PropertyToString( material-&gt;isOpaque() );</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="7" t="str">
+      <c r="C13" s="12"/>
+      <c r="D13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["AmbientColor"] = PropertyToString( material-&gt;getAmbientColor() );</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="7" t="str">
+      <c r="C14" s="12"/>
+      <c r="D14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["AmbientColorMap"] = PropertyToString( material-&gt;getAmbientColorMap() );</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="7" t="str">
+      <c r="C15" s="12"/>
+      <c r="D15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["AmbientStrength"] = PropertyToString( material-&gt;getAmbientStrength() );</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="7" t="str">
+      <c r="C16" s="12"/>
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["AmbientValueMap"] = PropertyToString( material-&gt;getAmbientValueMap() );</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="7" t="str">
+      <c r="C17" s="12"/>
+      <c r="D17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["BumpMap"] = PropertyToString( material-&gt;getBumpMap() );</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="7" t="str">
+      <c r="C18" s="12"/>
+      <c r="D18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["BumpMax"] = PropertyToString( material-&gt;getBumpMax() );</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="7" t="str">
+      <c r="C19" s="12"/>
+      <c r="D19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["BumpMin"] = PropertyToString( material-&gt;getBumpMin() );</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="7" t="str">
+      <c r="C20" s="12"/>
+      <c r="D20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["BumpStrength"] = PropertyToString( material-&gt;getBumpStrength() );</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="7" t="str">
+      <c r="C21" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DiffuseStrength"] = PropertyToString( material-&gt;getDiffuseStrength() );</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="7" t="str">
+      <c r="C22" s="12"/>
+      <c r="D22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DiffuseValueMap"] = PropertyToString( material-&gt;getDiffuseValueMap() );</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="7" t="str">
+      <c r="C23" s="12"/>
+      <c r="D23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DisplacementMap"] = PropertyToString( material-&gt;getDisplacementMap() );</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="7" t="str">
+      <c r="C24" s="12"/>
+      <c r="D24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DisplacementMax"] = PropertyToString( material-&gt;getDisplacementMax() );</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="7" t="str">
+      <c r="C25" s="12"/>
+      <c r="D25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DisplacementMin"] = PropertyToString( material-&gt;getDisplacementMin() );</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="7" t="str">
+      <c r="C26" s="12"/>
+      <c r="D26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["DisplacementStrength"] = PropertyToString( material-&gt;getDisplacementStrength() );</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="7" t="str">
+      <c r="C27" s="12"/>
+      <c r="D27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["GlossinessStrength"] = PropertyToString( material-&gt;getGlossinessStrength() );</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="7" t="str">
+      <c r="C28" s="12"/>
+      <c r="D28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["GlossinessValueMap"] = PropertyToString( material-&gt;getGlossinessValueMap() );</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="7" t="str">
+      <c r="C29" s="12"/>
+      <c r="D29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["HorizontalOffset"] = PropertyToString( material-&gt;getHorizontalOffset() );</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="7" t="str">
+      <c r="C30" s="12"/>
+      <c r="D30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["HorizontalTiles"] = PropertyToString( material-&gt;getHorizontalTiles() );</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="7" t="str">
+      <c r="C31" s="12"/>
+      <c r="D31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["IndexOfRefraction"] = PropertyToString( material-&gt;getIndexOfRefraction() );</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="7" t="str">
+      <c r="C32" s="12"/>
+      <c r="D32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["NormalValueMap"] = PropertyToString( material-&gt;getNormalValueMap() );</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="7" t="str">
+      <c r="C33" s="12"/>
+      <c r="D33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["ReflectionColor"] = PropertyToString( material-&gt;getReflectionColor() );</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="7" t="str">
+      <c r="C34" s="12"/>
+      <c r="D34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["ReflectionMap"] = PropertyToString( material-&gt;getReflectionMap() );</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="7" t="str">
+      <c r="C35" s="12"/>
+      <c r="D35" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["ReflectionStrength"] = PropertyToString( material-&gt;getReflectionStrength() );</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="7" t="str">
+      <c r="C36" s="12"/>
+      <c r="D36" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["ReflectionValueMap"] = PropertyToString( material-&gt;getReflectionValueMap() );</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="7" t="str">
+      <c r="C37" s="12"/>
+      <c r="D37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["RefractionColor"] = PropertyToString( material-&gt;getRefractionColor() );</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="7" t="str">
+      <c r="C38" s="12"/>
+      <c r="D38" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["RefractionColorMap"] = PropertyToString( material-&gt;getRefractionColorMap() );</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="7" t="str">
+      <c r="C39" s="12"/>
+      <c r="D39" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["RefractionStrength"] = PropertyToString( material-&gt;getRefractionStrength() );</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="7" t="str">
+      <c r="C40" s="12"/>
+      <c r="D40" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["RefractionValueMap"] = PropertyToString( material-&gt;getRefractionValueMap() );</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="7" t="str">
+      <c r="C41" s="12"/>
+      <c r="D41" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E41" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["SpecularColor"] = PropertyToString( material-&gt;getSpecularColor() );</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="7" t="str">
+      <c r="C42" s="12"/>
+      <c r="D42" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["SpecularColorMap"] = PropertyToString( material-&gt;getSpecularColorMap() );</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="7" t="str">
+      <c r="C43" s="12"/>
+      <c r="D43" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["SpecularStrength"] = PropertyToString( material-&gt;getSpecularStrength() );</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="7" t="str">
+      <c r="C44" s="12"/>
+      <c r="D44" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["SpecularValueMap"] = PropertyToString( material-&gt;getSpecularValueMap() );</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="7" t="str">
+      <c r="C45" s="12"/>
+      <c r="D45" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["SurfaceType"] = PropertyToString( material-&gt;getSurfaceType() );</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="7" t="str">
+      <c r="C46" s="12"/>
+      <c r="D46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["VerticalOffset"] = PropertyToString( material-&gt;getVerticalOffset() );</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="7" t="str">
+      <c r="C47" s="12"/>
+      <c r="D47" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["VerticalTiles"] = PropertyToString( material-&gt;getVerticalTiles() );</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7" t="str">
+      <c r="C48" s="12"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="str">
         <f t="shared" si="0"/>
         <v>properties["isMultThroughOpacity"] = PropertyToString( material-&gt;isMultThroughOpacity() );</v>
       </c>
@@ -2734,7 +2819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added managed MAX.NET plugin project to work in parallel with MaxScript/ManagedBridge Now collects scene data on start and removes geografted figures using the geograft list properties, same mechanic improves geograft figure selection speed Added support for exporting clothing
</commit_message>
<xml_diff>
--- a/Daz Materials.xlsx
+++ b/Daz Materials.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7995"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Daz Material Types" sheetId="1" r:id="rId1"/>
     <sheet name="Max Standard Material" sheetId="2" r:id="rId2"/>
-    <sheet name="Default to Standard Mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="231">
   <si>
     <t>GlossinessValueMap</t>
   </si>
@@ -159,21 +158,9 @@
     <t>VerticalOffset</t>
   </si>
   <si>
-    <t>Daz Material Method Prefix</t>
-  </si>
-  <si>
-    <t>get</t>
-  </si>
-  <si>
-    <t>Daz Material Code</t>
-  </si>
-  <si>
     <t>DzDefaultMaterial</t>
   </si>
   <si>
-    <t>When copying the below, copy into Word first to remove "" then into Notepad or Visual Studio, etc</t>
-  </si>
-  <si>
     <t>Our Alias</t>
   </si>
   <si>
@@ -712,27 +699,6 @@
   </si>
   <si>
     <t>Remember to apply a multiplier stage here because the Max shader doesn't utilise Diffuse Colour when a Diffuse Map is in use</t>
-  </si>
-  <si>
-    <t>Max Material Property</t>
-  </si>
-  <si>
-    <t>Our Daz Alias</t>
-  </si>
-  <si>
-    <t>Max Type</t>
-  </si>
-  <si>
-    <t>Conversion</t>
-  </si>
-  <si>
-    <t>PercentFromString</t>
-  </si>
-  <si>
-    <t>FloatFromString</t>
-  </si>
-  <si>
-    <t>ColourFromString</t>
   </si>
   <si>
     <t>Percent multiplied with diffuse colour (from map or DiffuseColor property)</t>
@@ -748,7 +714,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,15 +724,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -846,21 +803,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1164,15 +1119,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
     <col min="5" max="5" width="96.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
@@ -1185,28 +1140,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1215,12 +1164,9 @@
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="7" t="str">
-        <f>CONCATENATE("properties[""",B3,"""] = PropertyToString( material-&gt;",D3,A3,"() );")</f>
-        <v>properties["allowsAutoBake"] = PropertyToString( material-&gt;allowsAutoBake() );</v>
-      </c>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1229,14 +1175,9 @@
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="7" t="str">
-        <f t="shared" ref="E4:E48" si="0">CONCATENATE("properties[""",B4,"""] = PropertyToString( material-&gt;",D4,A4,"() );")</f>
-        <v>properties["BaseOpacity"] = PropertyToString( material-&gt;getBaseOpacity() );</v>
-      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1245,16 +1186,11 @@
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["ColorMap"] = PropertyToString( material-&gt;getColorMap() );</v>
-      </c>
+      <c r="C5" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1263,32 +1199,22 @@
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DiffuseColor"] = PropertyToString( material-&gt;getDiffuseColor() );</v>
-      </c>
+      <c r="C6" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["MaterialType"] = PropertyToString( material-&gt;getMaterialName() );</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1297,14 +1223,9 @@
       <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["NumGLMaps"] = PropertyToString( material-&gt;getNumGLMaps() );</v>
-      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1313,14 +1234,9 @@
       <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["OpacityMap"] = PropertyToString( material-&gt;getOpacityMap() );</v>
-      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1329,12 +1245,9 @@
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["isColorMappable"] = PropertyToString( material-&gt;isColorMappable() );</v>
-      </c>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1343,12 +1256,9 @@
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["isOpacityMappable"] = PropertyToString( material-&gt;isOpacityMappable() );</v>
-      </c>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1357,12 +1267,9 @@
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["isOpaque"] = PropertyToString( material-&gt;isOpaque() );</v>
-      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1371,14 +1278,9 @@
       <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["AmbientColor"] = PropertyToString( material-&gt;getAmbientColor() );</v>
-      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -1387,14 +1289,9 @@
       <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["AmbientColorMap"] = PropertyToString( material-&gt;getAmbientColorMap() );</v>
-      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -1403,14 +1300,9 @@
       <c r="B15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["AmbientStrength"] = PropertyToString( material-&gt;getAmbientStrength() );</v>
-      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1419,14 +1311,9 @@
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["AmbientValueMap"] = PropertyToString( material-&gt;getAmbientValueMap() );</v>
-      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1435,14 +1322,9 @@
       <c r="B17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["BumpMap"] = PropertyToString( material-&gt;getBumpMap() );</v>
-      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1451,14 +1333,9 @@
       <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["BumpMax"] = PropertyToString( material-&gt;getBumpMax() );</v>
-      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -1467,14 +1344,9 @@
       <c r="B19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["BumpMin"] = PropertyToString( material-&gt;getBumpMin() );</v>
-      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -1483,14 +1355,9 @@
       <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["BumpStrength"] = PropertyToString( material-&gt;getBumpStrength() );</v>
-      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -1499,16 +1366,11 @@
       <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DiffuseStrength"] = PropertyToString( material-&gt;getDiffuseStrength() );</v>
-      </c>
+      <c r="C21" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -1517,14 +1379,9 @@
       <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DiffuseValueMap"] = PropertyToString( material-&gt;getDiffuseValueMap() );</v>
-      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -1533,14 +1390,9 @@
       <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DisplacementMap"] = PropertyToString( material-&gt;getDisplacementMap() );</v>
-      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -1549,14 +1401,9 @@
       <c r="B24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DisplacementMax"] = PropertyToString( material-&gt;getDisplacementMax() );</v>
-      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -1565,14 +1412,9 @@
       <c r="B25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DisplacementMin"] = PropertyToString( material-&gt;getDisplacementMin() );</v>
-      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1581,14 +1423,9 @@
       <c r="B26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["DisplacementStrength"] = PropertyToString( material-&gt;getDisplacementStrength() );</v>
-      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -1597,14 +1434,9 @@
       <c r="B27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["GlossinessStrength"] = PropertyToString( material-&gt;getGlossinessStrength() );</v>
-      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -1613,14 +1445,9 @@
       <c r="B28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["GlossinessValueMap"] = PropertyToString( material-&gt;getGlossinessValueMap() );</v>
-      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
@@ -1629,14 +1456,9 @@
       <c r="B29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["HorizontalOffset"] = PropertyToString( material-&gt;getHorizontalOffset() );</v>
-      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1645,14 +1467,9 @@
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["HorizontalTiles"] = PropertyToString( material-&gt;getHorizontalTiles() );</v>
-      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
@@ -1661,14 +1478,9 @@
       <c r="B31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["IndexOfRefraction"] = PropertyToString( material-&gt;getIndexOfRefraction() );</v>
-      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -1677,14 +1489,9 @@
       <c r="B32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["NormalValueMap"] = PropertyToString( material-&gt;getNormalValueMap() );</v>
-      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -1693,14 +1500,9 @@
       <c r="B33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["ReflectionColor"] = PropertyToString( material-&gt;getReflectionColor() );</v>
-      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -1709,14 +1511,9 @@
       <c r="B34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["ReflectionMap"] = PropertyToString( material-&gt;getReflectionMap() );</v>
-      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
@@ -1725,14 +1522,9 @@
       <c r="B35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["ReflectionStrength"] = PropertyToString( material-&gt;getReflectionStrength() );</v>
-      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
@@ -1741,14 +1533,9 @@
       <c r="B36" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["ReflectionValueMap"] = PropertyToString( material-&gt;getReflectionValueMap() );</v>
-      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
@@ -1757,14 +1544,9 @@
       <c r="B37" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["RefractionColor"] = PropertyToString( material-&gt;getRefractionColor() );</v>
-      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -1773,14 +1555,9 @@
       <c r="B38" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["RefractionColorMap"] = PropertyToString( material-&gt;getRefractionColorMap() );</v>
-      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1789,14 +1566,9 @@
       <c r="B39" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["RefractionStrength"] = PropertyToString( material-&gt;getRefractionStrength() );</v>
-      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
@@ -1805,14 +1577,9 @@
       <c r="B40" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["RefractionValueMap"] = PropertyToString( material-&gt;getRefractionValueMap() );</v>
-      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -1821,14 +1588,9 @@
       <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["SpecularColor"] = PropertyToString( material-&gt;getSpecularColor() );</v>
-      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -1837,14 +1599,9 @@
       <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["SpecularColorMap"] = PropertyToString( material-&gt;getSpecularColorMap() );</v>
-      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
@@ -1853,14 +1610,9 @@
       <c r="B43" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["SpecularStrength"] = PropertyToString( material-&gt;getSpecularStrength() );</v>
-      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -1869,14 +1621,9 @@
       <c r="B44" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["SpecularValueMap"] = PropertyToString( material-&gt;getSpecularValueMap() );</v>
-      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -1885,14 +1632,9 @@
       <c r="B45" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["SurfaceType"] = PropertyToString( material-&gt;getSurfaceType() );</v>
-      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
@@ -1901,14 +1643,9 @@
       <c r="B46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["VerticalOffset"] = PropertyToString( material-&gt;getVerticalOffset() );</v>
-      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
@@ -1917,14 +1654,9 @@
       <c r="B47" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["VerticalTiles"] = PropertyToString( material-&gt;getVerticalTiles() );</v>
-      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
@@ -1933,12 +1665,9 @@
       <c r="B48" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>properties["isMultThroughOpacity"] = PropertyToString( material-&gt;isMultThroughOpacity() );</v>
-      </c>
+      <c r="E48" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1950,7 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -1965,1785 +1694,852 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
-  <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="F44" s="9"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="F52" s="9"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="F53" s="9"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="F55" s="9"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="F56" s="9"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" s="9"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="F58" s="9"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="F59" s="9"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="9"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="F63" s="9"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="F64" s="9"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="F65" s="9"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F66" s="9"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="F67" s="9"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="F68" s="9"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F69" s="9"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="F70" s="9"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C72" s="7"/>
-      <c r="F72" s="9"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C73" s="7"/>
-      <c r="F73" s="9"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C74" s="7"/>
-      <c r="F74" s="9"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C75" s="7"/>
-      <c r="F75" s="9"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C76" s="7"/>
-      <c r="F76" s="9"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C77" s="7"/>
-      <c r="F77" s="9"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C78" s="7"/>
-      <c r="F78" s="9"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F79" s="9"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F80" s="9"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F81" s="9"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" s="7"/>
-      <c r="F82" s="9"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" s="7"/>
-      <c r="F83" s="9"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" s="7"/>
-      <c r="F84" s="9"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C85" s="7"/>
-      <c r="F85" s="9"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C86" s="7"/>
-      <c r="F86" s="9"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C87" s="7"/>
-      <c r="F87" s="9"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F88" s="9"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F89" s="9"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C90" s="7"/>
-      <c r="F90" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Daz Material Types'!$B$3:$B$48</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>